<commit_message>
adjusted roadmap a bit and fixed template and excel for it
</commit_message>
<xml_diff>
--- a/Example-web 1.xlsx
+++ b/Example-web 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ellasartory/Desktop/tide-ws/tide-ws/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87BE7B40-E12B-A441-92DD-2576F3057416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7474E20-ED2C-5B47-82C0-C55322DA9068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="16960" xr2:uid="{8B004D9F-539D-2A46-9487-C8A7A0BAFD95}"/>
   </bookViews>
@@ -106,6 +106,61 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>148025</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE0D72B0-08EF-5E6D-4D53-106DA80545B0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12700" y="76200"/>
+          <a:ext cx="7772400" cy="4542225"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -428,7 +483,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -461,5 +516,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>